<commit_message>
[excel] ~ data update
</commit_message>
<xml_diff>
--- a/assets/data.xlsx
+++ b/assets/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\flutter\myTask\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535E411E-76B4-4565-AB5E-5B4143398D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6124AAE0-ABB1-44D2-9360-FC168C0E9259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22890" yWindow="2655" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Task index</t>
   </si>
@@ -46,10 +46,13 @@
     <t>Duration hours</t>
   </si>
   <si>
-    <t>duration minutes</t>
-  </si>
-  <si>
     <t>Duration days</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Duration minutes</t>
   </si>
 </sst>
 </file>
@@ -370,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,7 +390,7 @@
     <col min="8" max="8" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -398,19 +401,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>